<commit_message>
Updated code to have synonymous codon optimization instead of all codons freely
</commit_message>
<xml_diff>
--- a/tRNAShuffle/codonValues_RED20.xlsx
+++ b/tRNAShuffle/codonValues_RED20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akshay/Documents/TranslationDynamics/tRNAShuffle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5225C69A-0B89-9B44-AAB0-13E6C9D090BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C37D0B-8264-4D46-A765-28B58188F818}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20860" yWindow="1260" windowWidth="14760" windowHeight="15940" xr2:uid="{382C8ACD-C0AF-2440-A813-B863F0D59BAF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="106">
   <si>
     <t>GGA</t>
   </si>
@@ -222,10 +222,136 @@
     <t>GGG</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>*Used CUA instead of CUG</t>
   </si>
   <si>
     <t>*Used GGA instead of GGU</t>
+  </si>
+  <si>
+    <t>Gly</t>
+  </si>
+  <si>
+    <t>Glu</t>
+  </si>
+  <si>
+    <t>Asp</t>
+  </si>
+  <si>
+    <t>Val</t>
+  </si>
+  <si>
+    <t>Ala</t>
+  </si>
+  <si>
+    <t>Arg</t>
+  </si>
+  <si>
+    <t>Ser</t>
+  </si>
+  <si>
+    <t>Lys</t>
+  </si>
+  <si>
+    <t>Asn</t>
+  </si>
+  <si>
+    <t>Met</t>
+  </si>
+  <si>
+    <t>Ile</t>
+  </si>
+  <si>
+    <t>Thr</t>
+  </si>
+  <si>
+    <t>Trp</t>
+  </si>
+  <si>
+    <t>Cys</t>
+  </si>
+  <si>
+    <t>Stop</t>
+  </si>
+  <si>
+    <t>Tyr</t>
+  </si>
+  <si>
+    <t>Leu</t>
+  </si>
+  <si>
+    <t>Phe</t>
+  </si>
+  <si>
+    <t>Gln</t>
+  </si>
+  <si>
+    <t>His</t>
+  </si>
+  <si>
+    <t>Pro</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>U</t>
   </si>
 </sst>
 </file>
@@ -583,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19395223-B780-624B-8674-63EDE490B973}">
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -594,9 +720,15 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="2">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="E1" s="2">
         <v>2.36</v>
       </c>
@@ -609,9 +741,15 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="E2" s="2">
         <v>1.26</v>
       </c>
@@ -623,14 +761,20 @@
         <v>83.34</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="E3" s="2">
         <v>45.55</v>
       </c>
@@ -643,9 +787,15 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="E4" s="2">
         <v>34.17</v>
       </c>
@@ -663,9 +813,15 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="E5" s="2">
         <v>16.97</v>
       </c>
@@ -678,9 +834,15 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="E6" s="2">
         <v>57.86</v>
       </c>
@@ -694,9 +856,15 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="B7" s="2">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="E7" s="2">
         <v>19.27</v>
       </c>
@@ -709,9 +877,15 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="B8" s="2">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="E8" s="2">
         <v>33.74</v>
       </c>
@@ -725,9 +899,15 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="B9" s="2">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="E9" s="2">
         <v>14.98</v>
       </c>
@@ -740,9 +920,15 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="B10" s="2">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="E10" s="2">
         <v>22.31</v>
       </c>
@@ -755,9 +941,15 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="E11" s="2">
         <v>43.18</v>
       </c>
@@ -770,9 +962,15 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="B12" s="2">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="E12" s="2">
         <v>7.67</v>
       </c>
@@ -786,9 +984,15 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="B13" s="2">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="E13" s="2">
         <v>24.11</v>
       </c>
@@ -801,9 +1005,15 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="B14" s="2">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="E14" s="2">
         <v>24.87</v>
       </c>
@@ -817,9 +1027,15 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="B15" s="2">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="E15" s="2">
         <v>39.49</v>
       </c>
@@ -832,9 +1048,15 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="B16" s="2">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="E16" s="2">
         <v>11.81</v>
       </c>
@@ -847,9 +1069,15 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="B17" s="2">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="E17" s="2">
         <v>0.03</v>
       </c>
@@ -862,9 +1090,15 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="B18" s="2">
+        <v>17</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="E18" s="2">
         <v>0.63</v>
       </c>
@@ -877,9 +1111,15 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="B19" s="2">
+        <v>18</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="E19" s="2">
         <v>2.19</v>
       </c>
@@ -892,9 +1132,15 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="B20" s="2">
+        <v>19</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="E20" s="2">
         <v>9.31</v>
       </c>
@@ -907,9 +1153,15 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="B21" s="2">
+        <v>20</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="E21" s="2">
         <v>17.22</v>
       </c>
@@ -922,9 +1174,15 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="B22" s="2">
+        <v>21</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="E22" s="2">
         <v>55.01</v>
       </c>
@@ -938,9 +1196,15 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="B23" s="2">
+        <v>22</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="E23" s="2">
         <v>5.61</v>
       </c>
@@ -953,9 +1217,15 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="B24" s="2">
+        <v>23</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="E24" s="2">
         <v>29.21</v>
       </c>
@@ -969,9 +1239,15 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="B25" s="2">
+        <v>24</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="E25" s="2">
         <v>21.67</v>
       </c>
@@ -985,9 +1261,15 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+      <c r="B26" s="2">
+        <v>25</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="E26" s="2">
         <v>0.52</v>
       </c>
@@ -1000,9 +1282,15 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="B27" s="2">
+        <v>26</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="E27" s="2">
         <v>15.79</v>
       </c>
@@ -1015,9 +1303,15 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
+      <c r="B28" s="2">
+        <v>27</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="E28" s="2">
         <v>43.86</v>
       </c>
@@ -1031,9 +1325,15 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+      <c r="B29" s="2">
+        <v>28</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="E29" s="2">
         <v>4.17</v>
       </c>
@@ -1046,9 +1346,15 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
+      <c r="B30" s="2">
+        <v>29</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="E30" s="2">
         <v>2.61</v>
       </c>
@@ -1061,9 +1367,15 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
+      <c r="B31" s="2">
+        <v>30</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="E31" s="2">
         <v>20.64</v>
       </c>
@@ -1076,9 +1388,15 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+      <c r="B32" s="2">
+        <v>31</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="E32" s="2">
         <v>26.7</v>
       </c>
@@ -1092,9 +1410,15 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
+      <c r="B33" s="2">
+        <v>32</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="E33" s="2">
         <v>7.03</v>
       </c>
@@ -1108,9 +1432,15 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
+      <c r="B34" s="2">
+        <v>33</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="E34" s="2">
         <v>0.19</v>
       </c>
@@ -1124,9 +1454,15 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
+      <c r="B35" s="2">
+        <v>34</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="E35" s="2">
         <v>2.76</v>
       </c>
@@ -1139,9 +1475,15 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
+      <c r="B36" s="2">
+        <v>35</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="E36" s="2">
         <v>3.81</v>
       </c>
@@ -1155,9 +1497,15 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
+      <c r="B37" s="2">
+        <v>36</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="E37" s="2">
         <v>6.72</v>
       </c>
@@ -1170,9 +1518,15 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
+      <c r="B38" s="2">
+        <v>37</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="E38" s="2">
         <v>16.52</v>
       </c>
@@ -1186,9 +1540,15 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
+      <c r="B39" s="2">
+        <v>38</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="E39" s="2">
         <v>4.2699999999999996</v>
       </c>
@@ -1201,9 +1561,15 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
+      <c r="B40" s="2">
+        <v>39</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="E40" s="2">
         <v>2.73</v>
       </c>
@@ -1216,9 +1582,15 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
+      <c r="B41" s="2">
+        <v>40</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="E41" s="2">
         <v>7.92</v>
       </c>
@@ -1231,9 +1603,15 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
+      <c r="B42" s="2">
+        <v>41</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="E42" s="2">
         <v>23.25</v>
       </c>
@@ -1247,9 +1625,15 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
+      <c r="B43" s="2">
+        <v>42</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="E43" s="2">
         <v>2.5099999999999998</v>
       </c>
@@ -1262,9 +1646,15 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
+      <c r="B44" s="2">
+        <v>43</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="E44" s="2">
         <v>1.98</v>
       </c>
@@ -1272,15 +1662,21 @@
         <v>42</v>
       </c>
       <c r="G44" s="1">
-        <f>E45+E46+E44+E43</f>
-        <v>32.5</v>
+        <f>E45+E46+E44+E43+E19+E20</f>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
+      <c r="B45" s="2">
+        <v>44</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="E45" s="2">
         <v>16.329999999999998</v>
       </c>
@@ -1293,9 +1689,15 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
+      <c r="B46" s="2">
+        <v>45</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="E46" s="2">
         <v>11.68</v>
       </c>
@@ -1308,9 +1710,15 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
+      <c r="B47" s="2">
+        <v>46</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="E47" s="2">
         <v>0.62</v>
       </c>
@@ -1323,9 +1731,15 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
+      <c r="B48" s="2">
+        <v>47</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="E48" s="2">
         <v>0.67</v>
       </c>
@@ -1338,9 +1752,15 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
+      <c r="B49" s="2">
+        <v>48</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="E49" s="2">
         <v>43.82</v>
       </c>
@@ -1354,9 +1774,15 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
+      <c r="B50" s="2">
+        <v>49</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="E50" s="2">
         <v>20.59</v>
       </c>
@@ -1369,9 +1795,15 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
+      <c r="B51" s="2">
+        <v>50</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="E51" s="2">
         <v>27.28</v>
       </c>
@@ -1385,9 +1817,15 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
+      <c r="B52" s="2">
+        <v>51</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="E52" s="2">
         <v>7.01</v>
       </c>
@@ -1400,9 +1838,15 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
+      <c r="B53" s="2">
+        <v>52</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E53" s="2">
         <v>6.78</v>
       </c>
@@ -1415,9 +1859,15 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
+      <c r="B54" s="2">
+        <v>53</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E54" s="2">
         <v>14.21</v>
       </c>
@@ -1431,9 +1881,15 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
+      <c r="B55" s="2">
+        <v>54</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="E55" s="2">
         <v>60.75</v>
       </c>
@@ -1446,9 +1902,15 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
+      <c r="B56" s="2">
+        <v>55</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="E56" s="2">
         <v>0.82</v>
       </c>
@@ -1460,14 +1922,20 @@
         <v>76.52</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
+      <c r="B57" s="2">
+        <v>56</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="E57" s="2">
         <v>3.86</v>
       </c>
@@ -1480,9 +1948,15 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
+      <c r="B58" s="2">
+        <v>57</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="E58" s="2">
         <v>4.09</v>
       </c>
@@ -1495,9 +1969,15 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
+      <c r="B59" s="2">
+        <v>58</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="E59" s="2">
         <v>28.82</v>
       </c>
@@ -1511,9 +1991,15 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
+      <c r="B60" s="2">
+        <v>59</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="E60" s="2">
         <v>5.18</v>
       </c>
@@ -1526,9 +2012,15 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
+      <c r="B61" s="2">
+        <v>60</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="E61" s="2">
         <v>4.38</v>
       </c>
@@ -1541,9 +2033,15 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
+      <c r="B62" s="2">
+        <v>61</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="E62" s="2">
         <v>1.0900000000000001</v>
       </c>

</xml_diff>